<commit_message>
update 23.222 nyan nyan
</commit_message>
<xml_diff>
--- a/data/Dialog/Drama/ineien.xlsx
+++ b/data/Dialog/Drama/ineien.xlsx
@@ -8,7 +8,7 @@
     <workbookView windowWidth="16384" windowHeight="8192" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="fiama" sheetId="1" r:id="rId2"/>
+    <sheet name="fiama" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcMode="auto" fullCalcOnLoad="0" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.001" fullPrecision="1" calcCompleted="0" calcOnSave="0" concurrentCalc="0" forceFullCalc="0"/>
   <extLst>
@@ -126,7 +126,7 @@
     <t xml:space="preserve">Willow is a fort in the territory of Mysilia. 150 years ago when I was given this land, I named it Lothria. It means "Promised Land" in the old Elean language. But for some time now, people have called the fort by the name of the willow trees that surround it. Now I call it Willow, too.</t>
   </si>
   <si>
-    <t xml:space="preserve">…かつて、このウィロウは、ミシリアの掲げる人間とエレアの共存の象徴だった。しかし、二十年前の戦争で互いの関係にきしみが生じて以来、ウィロウの灯りもまた、照らす場所を失いくすぶっている。</t>
+    <t xml:space="preserve">…かつて、このウィロウは、ミシリアの掲げる人間とエレアの共存の象徴だった。しかし、先の戦争で互いの関係にきしみが生じて以来、ウィロウの灯りもまた、照らす場所を失いくすぶっている。</t>
   </si>
   <si>
     <t xml:space="preserve">...In the past, Willow was the symbol of the coexistence of humans and Elea that Mysilia upheld. However, when the last war caused the relationship between the two races to be strained, Willow's light has also lost its place to shine and has been smoldering since then.</t>
@@ -347,6 +347,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
@@ -357,7 +463,7 @@
     <sheetView tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K28" sqref="K28"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.8"/>
@@ -554,7 +660,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" ht="137.3">
+    <row r="27" ht="64.15">
       <c r="H27" s="1">
         <v>6</v>
       </c>

</xml_diff>